<commit_message>
added ESR type 2 cap
</commit_message>
<xml_diff>
--- a/excel/Trades/TraderPortfolios.xlsx
+++ b/excel/Trades/TraderPortfolios.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/NGEEHUNG/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/NGEEHUNG/DEV/proUBS/excel/Trades/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="73">
   <si>
     <t>Symbol</t>
   </si>
@@ -246,6 +246,9 @@
   </si>
   <si>
     <t>Lucy</t>
+  </si>
+  <si>
+    <t>9..75</t>
   </si>
 </sst>
 </file>
@@ -1126,7 +1129,7 @@
   <dimension ref="A1:J32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="J29" sqref="J29"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -1552,8 +1555,8 @@
       <c r="H13" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="I13" s="1">
-        <v>9.75</v>
+      <c r="I13" s="1" t="s">
+        <v>72</v>
       </c>
       <c r="J13" s="1" t="s">
         <v>68</v>

</xml_diff>

<commit_message>
fixed the error for new RMS finding
</commit_message>
<xml_diff>
--- a/excel/Trades/TraderPortfolios.xlsx
+++ b/excel/Trades/TraderPortfolios.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/NGEEHUNG/DEV/proUBS/excel/Trades/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/NGEEHUNG/DEV/proUBS/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15,7 +15,7 @@
     <sheet name="Portfolio_20170410" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Portfolio_20170410!$A$1:$I$29</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Portfolio_20170410!$A$1:$I$17</definedName>
   </definedNames>
   <calcPr calcId="0" concurrentCalc="0"/>
   <extLst>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="57">
   <si>
     <t>Symbol</t>
   </si>
@@ -38,217 +38,169 @@
     <t>SEHK</t>
   </si>
   <si>
-    <t>OTC</t>
+    <t>0003.HK</t>
+  </si>
+  <si>
+    <t>0004.HK</t>
+  </si>
+  <si>
+    <t>0005.HK</t>
+  </si>
+  <si>
+    <t>0006.HK</t>
+  </si>
+  <si>
+    <t>0011.HK</t>
+  </si>
+  <si>
+    <t>0016.HK</t>
+  </si>
+  <si>
+    <t>0017.HK</t>
+  </si>
+  <si>
+    <t>0023.HK</t>
+  </si>
+  <si>
+    <t>0066.HK</t>
+  </si>
+  <si>
+    <t>0083.HK</t>
+  </si>
+  <si>
+    <t>0135.HK</t>
+  </si>
+  <si>
+    <t>0151.HK</t>
+  </si>
+  <si>
+    <t>0175.HK</t>
+  </si>
+  <si>
+    <t>0267.HK</t>
+  </si>
+  <si>
+    <t>0388.HK</t>
+  </si>
+  <si>
+    <t>0700.HK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Exchange Markets </t>
+  </si>
+  <si>
+    <t>Position</t>
+  </si>
+  <si>
+    <t>Undelying Product</t>
+  </si>
+  <si>
+    <t>Reuter RIC</t>
+  </si>
+  <si>
+    <t>6436557 Sedol</t>
+  </si>
+  <si>
+    <t>6435576 Sedol</t>
+  </si>
+  <si>
+    <t>6158163 Sedol</t>
+  </si>
+  <si>
+    <t>6435327 Sedol</t>
+  </si>
+  <si>
+    <t>6408374 Sedol</t>
+  </si>
+  <si>
+    <t>6859927 Sedol</t>
+  </si>
+  <si>
+    <t>6633767 Sedol</t>
+  </si>
+  <si>
+    <t>6075648 Sedol</t>
+  </si>
+  <si>
+    <t>6290054 Sedol</t>
+  </si>
+  <si>
+    <t>6810429 Sedol</t>
+  </si>
+  <si>
+    <t>6340078 Sedol</t>
+  </si>
+  <si>
+    <t>B2Q14Z3 Sedol</t>
+  </si>
+  <si>
+    <t>6531827 Sedol</t>
+  </si>
+  <si>
+    <t>6196152 Sedol</t>
+  </si>
+  <si>
+    <t>6267359 Sedol</t>
+  </si>
+  <si>
+    <t>BMMV2K8 Sedol</t>
+  </si>
+  <si>
+    <t>PORT_SEHK</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>Hong Kong</t>
+  </si>
+  <si>
+    <t>BLOOMBERG Sedol</t>
+  </si>
+  <si>
+    <t>Internal Price Quote</t>
+  </si>
+  <si>
+    <t>Portfolio</t>
+  </si>
+  <si>
+    <t>Trader Name</t>
+  </si>
+  <si>
+    <t>Hagen</t>
   </si>
   <si>
     <t>0002.HK</t>
   </si>
   <si>
-    <t>0003.HK</t>
-  </si>
-  <si>
-    <t>0004.HK</t>
-  </si>
-  <si>
-    <t>0005.HK</t>
-  </si>
-  <si>
-    <t>0006.HK</t>
-  </si>
-  <si>
-    <t>0011.HK</t>
+    <t>6097017 Sedol</t>
+  </si>
+  <si>
+    <t>Caden</t>
   </si>
   <si>
     <t>0012.HK</t>
   </si>
   <si>
-    <t>0016.HK</t>
-  </si>
-  <si>
-    <t>0017.HK</t>
+    <t>6420538 Sedol</t>
   </si>
   <si>
     <t>0019.HK</t>
   </si>
   <si>
-    <t>0023.HK</t>
-  </si>
-  <si>
-    <t>0066.HK</t>
-  </si>
-  <si>
-    <t>0083.HK</t>
+    <t>6867748 Sedol</t>
   </si>
   <si>
     <t>0101.HK</t>
   </si>
   <si>
-    <t>0135.HK</t>
-  </si>
-  <si>
-    <t>0144.HK</t>
-  </si>
-  <si>
-    <t>0151.HK</t>
-  </si>
-  <si>
-    <t>0175.HK</t>
-  </si>
-  <si>
-    <t>0267.HK</t>
+    <t>6030506 Sedol</t>
   </si>
   <si>
     <t>0293.HK</t>
   </si>
   <si>
-    <t>0388.HK</t>
-  </si>
-  <si>
-    <t>0700.HK</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Exchange Markets </t>
-  </si>
-  <si>
-    <t>Position</t>
-  </si>
-  <si>
-    <t>Undelying Product</t>
-  </si>
-  <si>
-    <t>Reuter RIC</t>
-  </si>
-  <si>
-    <t>6097017 Sedol</t>
-  </si>
-  <si>
-    <t>6436557 Sedol</t>
-  </si>
-  <si>
-    <t>6435576 Sedol</t>
-  </si>
-  <si>
-    <t>6158163 Sedol</t>
-  </si>
-  <si>
-    <t>6435327 Sedol</t>
-  </si>
-  <si>
-    <t>6408374 Sedol</t>
-  </si>
-  <si>
-    <t>6420538 Sedol</t>
-  </si>
-  <si>
-    <t>6859927 Sedol</t>
-  </si>
-  <si>
-    <t>6633767 Sedol</t>
-  </si>
-  <si>
-    <t>6867748 Sedol</t>
-  </si>
-  <si>
-    <t>6075648 Sedol</t>
-  </si>
-  <si>
-    <t>6290054 Sedol</t>
-  </si>
-  <si>
-    <t>6810429 Sedol</t>
-  </si>
-  <si>
-    <t>6030506 Sedol</t>
-  </si>
-  <si>
-    <t>6340078 Sedol</t>
-  </si>
-  <si>
-    <t>6416139 Sedol</t>
-  </si>
-  <si>
-    <t>B2Q14Z3 Sedol</t>
-  </si>
-  <si>
-    <t>6531827 Sedol</t>
-  </si>
-  <si>
-    <t>6196152 Sedol</t>
-  </si>
-  <si>
     <t>6179755 Sedol</t>
-  </si>
-  <si>
-    <t>6267359 Sedol</t>
-  </si>
-  <si>
-    <t>BMMV2K8 Sedol</t>
-  </si>
-  <si>
-    <t>PORT_SEHK</t>
-  </si>
-  <si>
-    <t>PORT_OTC</t>
-  </si>
-  <si>
-    <t>Over-the-counter</t>
-  </si>
-  <si>
-    <t>Country</t>
-  </si>
-  <si>
-    <t>Hong Kong</t>
-  </si>
-  <si>
-    <t>BLOOMBERG Sedol</t>
-  </si>
-  <si>
-    <t>Internal Price Quote</t>
-  </si>
-  <si>
-    <t>Portfolio</t>
-  </si>
-  <si>
-    <t>0005_BULL_ELN</t>
-  </si>
-  <si>
-    <t>0175_BULL_ELN</t>
-  </si>
-  <si>
-    <t>0700_BULL_ELN</t>
-  </si>
-  <si>
-    <t>0016.HK_CALL_SPREAD</t>
-  </si>
-  <si>
-    <t>0016.HK_PUT_SPREAD</t>
-  </si>
-  <si>
-    <t>0023_CALL</t>
-  </si>
-  <si>
-    <t>0144_PUT</t>
-  </si>
-  <si>
-    <t>Trader Name</t>
-  </si>
-  <si>
-    <t>Jack</t>
-  </si>
-  <si>
-    <t>John</t>
-  </si>
-  <si>
-    <t>Jim</t>
-  </si>
-  <si>
-    <t>Tom</t>
-  </si>
-  <si>
-    <t>Lucy</t>
-  </si>
-  <si>
-    <t>9..75</t>
   </si>
 </sst>
 </file>
@@ -817,6 +769,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1126,13 +1081,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J32"/>
+  <dimension ref="A1:J38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="32.6640625" style="1" customWidth="1"/>
     <col min="2" max="2" width="18.6640625" style="1" customWidth="1"/>
@@ -1143,7 +1098,7 @@
     <col min="7" max="7" width="15.83203125" style="1" customWidth="1"/>
     <col min="8" max="8" width="18.1640625" style="1" customWidth="1"/>
     <col min="9" max="9" width="19.5" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="8.83203125" style="1"/>
+    <col min="10" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.15">
@@ -1151,194 +1106,194 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>58</v>
+        <v>43</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>54</v>
+        <v>39</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>56</v>
+        <v>41</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>57</v>
+        <v>42</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>66</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>55</v>
+        <v>40</v>
       </c>
       <c r="F2" s="1">
-        <v>-90227</v>
+        <v>-7245</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="I2" s="1">
-        <v>82.45</v>
+        <v>15.9</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>67</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>55</v>
+        <v>40</v>
       </c>
       <c r="F3" s="1">
-        <v>-59462</v>
+        <v>-93204</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="I3" s="1">
-        <v>15.9</v>
+        <v>66.7</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>67</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F4" s="1">
+        <v>9023</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I4" s="1">
+        <v>63.4</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="F4" s="1">
-        <v>52386</v>
-      </c>
-      <c r="G4" s="1" t="s">
+      <c r="C5" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F5" s="1">
+        <v>6820</v>
+      </c>
+      <c r="G5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H4" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="I4" s="1">
-        <v>66.7</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="1" t="s">
+      <c r="H5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I5" s="1">
+        <v>68.8</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A6" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="F5" s="1">
-        <v>-67902</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="I5" s="1">
-        <v>63.4</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A6" s="1" t="s">
-        <v>59</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="F6" s="1">
-        <v>-25194</v>
+        <v>8294</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>6</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="I6" s="1">
-        <v>63.4</v>
+        <v>157.69999999999999</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.15">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
@@ -1346,28 +1301,28 @@
         <v>7</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>1</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>55</v>
+        <v>40</v>
       </c>
       <c r="F7" s="1">
-        <v>-20049</v>
+        <v>-7453</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>7</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="I7" s="1">
-        <v>68.8</v>
+        <v>117.6</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>67</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1378,28 +1333,28 @@
         <v>8</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>1</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>55</v>
+        <v>40</v>
       </c>
       <c r="F8" s="1">
-        <v>-52283</v>
+        <v>-12893</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>8</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="I8" s="1">
-        <v>157.69999999999999</v>
+        <v>9.75</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>67</v>
+        <v>45</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1410,673 +1365,960 @@
         <v>9</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>1</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>55</v>
+        <v>40</v>
       </c>
       <c r="F9" s="1">
-        <v>8017</v>
+        <v>28304</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>9</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="I9" s="1">
-        <v>49.6</v>
+        <v>32.15</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>67</v>
+        <v>45</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="1" t="s">
-        <v>62</v>
+        <v>10</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="F10" s="1">
-        <v>18089</v>
+        <v>-63724</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>10</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="I10" s="1">
-        <v>117.6</v>
+        <v>44.45</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>69</v>
+        <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="1" t="s">
-        <v>63</v>
+        <v>11</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="F11" s="1">
-        <v>-64032</v>
+        <v>73292</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="I11" s="1">
-        <v>117.6</v>
+        <v>13.48</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>68</v>
+        <v>45</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>1</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>55</v>
+        <v>40</v>
       </c>
       <c r="F12" s="1">
-        <v>12171</v>
+        <v>-81891</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="I12" s="1">
-        <v>117.6</v>
+        <v>7.95</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>68</v>
+        <v>45</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>1</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>55</v>
+        <v>40</v>
       </c>
       <c r="F13" s="1">
-        <v>-71146</v>
+        <v>-283</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="I13" s="1" t="s">
-        <v>72</v>
+        <v>33</v>
+      </c>
+      <c r="I13" s="1">
+        <v>5.6</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>68</v>
+        <v>45</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>1</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>55</v>
+        <v>40</v>
       </c>
       <c r="F14" s="1">
-        <v>35896</v>
+        <v>72839</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="I14" s="1">
-        <v>78.099999999999994</v>
+        <v>10.5</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>68</v>
+        <v>45</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>1</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>55</v>
+        <v>40</v>
       </c>
       <c r="F15" s="1">
-        <v>61712</v>
+        <v>13445</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="I15" s="1">
-        <v>32.15</v>
+        <v>11.02</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>68</v>
+        <v>45</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="1" t="s">
-        <v>64</v>
+        <v>16</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="F16" s="1">
-        <v>-15359</v>
+        <v>1237</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="I16" s="1">
-        <v>32.15</v>
+        <v>195.5</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>68</v>
+        <v>45</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>1</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>55</v>
+        <v>40</v>
       </c>
       <c r="F17" s="1">
-        <v>15030</v>
+        <v>78834</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="I17" s="1">
-        <v>44.45</v>
+        <v>226.4</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A18" s="1" t="s">
-        <v>15</v>
+        <v>46</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>15</v>
+        <v>46</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>1</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>55</v>
+        <v>40</v>
       </c>
       <c r="F18" s="1">
-        <v>30056</v>
+        <v>-82272</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>15</v>
+        <v>46</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="I18" s="1">
-        <v>13.48</v>
+        <v>82.45</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>68</v>
+        <v>48</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A19" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F19" s="1">
+        <v>59642</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I19" s="1">
+        <v>15.9</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A20" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F20" s="1">
+        <v>-38267</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I20" s="1">
+        <v>66.7</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A21" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F21" s="1">
+        <v>56812</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I21" s="1">
+        <v>63.4</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A22" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F22" s="1">
+        <v>20049</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I22" s="1">
+        <v>68.8</v>
+      </c>
+      <c r="J22" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A23" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F23" s="1">
+        <v>-52283</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I23" s="1">
+        <v>157.69999999999999</v>
+      </c>
+      <c r="J23" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A24" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F24" s="1">
+        <v>8017</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="I24" s="1">
+        <v>49.6</v>
+      </c>
+      <c r="J24" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A25" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F25" s="1">
+        <v>-12171</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I25" s="1">
+        <v>117.6</v>
+      </c>
+      <c r="J25" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A26" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F26" s="1">
+        <v>-71146</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I26" s="1">
+        <v>9.75</v>
+      </c>
+      <c r="J26" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A27" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F27" s="1">
+        <v>21786</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="I27" s="1">
+        <v>78.099999999999994</v>
+      </c>
+      <c r="J27" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A28" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F28" s="1">
+        <v>61712</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I28" s="1">
+        <v>32.15</v>
+      </c>
+      <c r="J28" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A29" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F29" s="1">
+        <v>15030</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I29" s="1">
+        <v>44.45</v>
+      </c>
+      <c r="J29" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A30" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F30" s="1">
+        <v>30056</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I30" s="1">
+        <v>13.48</v>
+      </c>
+      <c r="J30" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A31" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F31" s="1">
+        <v>-80667</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="I31" s="1">
+        <v>20.65</v>
+      </c>
+      <c r="J31" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A32" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F32" s="1">
+        <v>-95033</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H32" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I32" s="1">
+        <v>7.95</v>
+      </c>
+      <c r="J32" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A33" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F33" s="1">
+        <v>-47673</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H33" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I33" s="1">
+        <v>5.6</v>
+      </c>
+      <c r="J33" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A34" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F34" s="1">
+        <v>96514</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H34" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I34" s="1">
+        <v>10.5</v>
+      </c>
+      <c r="J34" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A35" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F35" s="1">
+        <v>88110</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H35" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="I35" s="1">
+        <v>11.02</v>
+      </c>
+      <c r="J35" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A36" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F36" s="1">
+        <v>7812</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="H36" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="I36" s="1">
+        <v>11.16</v>
+      </c>
+      <c r="J36" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A37" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B37" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="F19" s="1">
-        <v>-70668</v>
-      </c>
-      <c r="G19" s="1" t="s">
+      <c r="C37" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F37" s="1">
+        <v>92775</v>
+      </c>
+      <c r="G37" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="H19" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="I19" s="1">
-        <v>20.65</v>
-      </c>
-      <c r="J19" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A20" s="1" t="s">
+      <c r="H37" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="I37" s="1">
+        <v>195.5</v>
+      </c>
+      <c r="J37" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A38" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B38" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="F20" s="1">
-        <v>-95033</v>
-      </c>
-      <c r="G20" s="1" t="s">
+      <c r="C38" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F38" s="1">
+        <v>31601</v>
+      </c>
+      <c r="G38" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="H20" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="I20" s="1">
-        <v>7.95</v>
-      </c>
-      <c r="J20" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A21" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="F21" s="1">
-        <v>-53110</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="H21" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="I21" s="1">
-        <v>22.4</v>
-      </c>
-      <c r="J21" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A22" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="F22" s="1">
-        <v>-47673</v>
-      </c>
-      <c r="G22" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="H22" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="I22" s="1">
-        <v>5.6</v>
-      </c>
-      <c r="J22" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A23" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="F23" s="1">
-        <v>96514</v>
-      </c>
-      <c r="G23" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="H23" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="I23" s="1">
-        <v>10.5</v>
-      </c>
-      <c r="J23" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A24" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="F24" s="1">
-        <v>-16761</v>
-      </c>
-      <c r="G24" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="H24" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="I24" s="1">
-        <v>10.5</v>
-      </c>
-      <c r="J24" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A25" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="F25" s="1">
-        <v>88110</v>
-      </c>
-      <c r="G25" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="H25" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="I25" s="1">
-        <v>11.02</v>
-      </c>
-      <c r="J25" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A26" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="F26" s="1">
-        <v>45200</v>
-      </c>
-      <c r="G26" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="H26" s="1" t="s">
+      <c r="H38" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="I38" s="1">
+        <v>226.4</v>
+      </c>
+      <c r="J38" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="I26" s="1">
-        <v>11.16</v>
-      </c>
-      <c r="J26" s="1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A27" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="F27" s="1">
-        <v>92775</v>
-      </c>
-      <c r="G27" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="H27" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="I27" s="1">
-        <v>195.5</v>
-      </c>
-      <c r="J27" s="1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A28" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="F28" s="1">
-        <v>31601</v>
-      </c>
-      <c r="G28" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="H28" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="I28" s="1">
-        <v>226.4</v>
-      </c>
-      <c r="J28" s="1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A29" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="F29" s="1">
-        <v>54335</v>
-      </c>
-      <c r="G29" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="H29" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="I29" s="1">
-        <v>226.4</v>
-      </c>
-      <c r="J29" s="1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.15"/>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:I29"/>
+  <autoFilter ref="A1:I17"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>